<commit_message>
Ejercicios 1 al 10
</commit_message>
<xml_diff>
--- a/Fisica/tp1 fisica.xlsx
+++ b/Fisica/tp1 fisica.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Descargas\UTN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxi Bernard\Documents\UTN\Fisica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C0E86-21CA-4B35-8EE9-9DAFB0165D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121C8131-3383-44D0-83D4-B3CF1A41CE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49395162-4F31-4427-BA9A-05B966F1B272}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Altura</t>
   </si>
@@ -82,6 +82,21 @@
   <si>
     <t>Frecuencia</t>
   </si>
+  <si>
+    <t>25,36-25,38</t>
+  </si>
+  <si>
+    <t>25,33-25,35</t>
+  </si>
+  <si>
+    <t>25,30-25,32</t>
+  </si>
+  <si>
+    <t>25,29-25,31</t>
+  </si>
+  <si>
+    <t>25,26-25,28</t>
+  </si>
 </sst>
 </file>
 
@@ -309,6 +324,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,10 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,79 +1000,48 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$26:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:f>Sheet1!$F$53:$F$57</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25.26</c:v>
+                  <c:v>25,26-25,28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.27</c:v>
+                  <c:v>25,29-25,31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.3</c:v>
+                  <c:v>25,30-25,32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.31</c:v>
+                  <c:v>25,33-25,35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.34</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25.37</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.38</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>25,36-25,38</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$26:$D$35</c:f>
+              <c:f>Sheet1!$G$53:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1102,79 +1086,48 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$26:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+            <c:strRef>
+              <c:f>Sheet1!$F$53:$F$57</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25.26</c:v>
+                  <c:v>25,26-25,28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.27</c:v>
+                  <c:v>25,29-25,31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.3</c:v>
+                  <c:v>25,30-25,32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.31</c:v>
+                  <c:v>25,33-25,35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.34</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25.37</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.38</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>25,36-25,38</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$26:$D$35</c:f>
+              <c:f>Sheet1!$G$53:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,7 +1135,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-297B-4D6B-92EC-F5A25B6A26EA}"/>
+              <c16:uniqueId val="{00000001-581C-400F-A883-879CB48A9112}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1261,7 +1214,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2595,15 +2548,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>379344</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>436494</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>105604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2931,10 +2884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD147F1C-78F0-45B7-9B02-6957FF89D9A8}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,25 +2906,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
+      <c r="H1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="27"/>
-      <c r="S1" s="25" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="31"/>
+      <c r="S1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="27"/>
+      <c r="T1" s="31"/>
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="3:21" x14ac:dyDescent="0.25">
@@ -3025,11 +2978,11 @@
       <c r="E3" s="10">
         <v>25.34</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="23">
         <f>D3-$H$3</f>
         <v>8.3333333333332149E-2</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="23">
         <f>E3-$I$3</f>
         <v>1.0000000000001563E-2</v>
       </c>
@@ -3083,11 +3036,11 @@
       <c r="E4" s="10">
         <v>25.33</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="23">
         <f t="shared" ref="F4:F14" si="0">D4-$H$3</f>
         <v>8.3333333333332149E-2</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="23">
         <f t="shared" ref="G4:G14" si="1">E4-$I$3</f>
         <v>0</v>
       </c>
@@ -3102,11 +3055,11 @@
       <c r="E5" s="10">
         <v>25.31</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
         <v>3.3333333333331439E-2</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="23">
         <f t="shared" si="1"/>
         <v>-1.9999999999999574E-2</v>
       </c>
@@ -3121,11 +3074,11 @@
       <c r="E6" s="10">
         <v>25.32</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="23">
         <f t="shared" si="0"/>
         <v>-0.11666666666666714</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="23">
         <f t="shared" si="1"/>
         <v>-9.9999999999980105E-3</v>
       </c>
@@ -3140,11 +3093,11 @@
       <c r="E7" s="10">
         <v>25.38</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="23">
         <f t="shared" si="0"/>
         <v>3.3333333333331439E-2</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="23">
         <f t="shared" si="1"/>
         <v>5.0000000000000711E-2</v>
       </c>
@@ -3159,11 +3112,11 @@
       <c r="E8" s="10">
         <v>25.3</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="23">
         <f t="shared" si="0"/>
         <v>8.3333333333332149E-2</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="23">
         <f t="shared" si="1"/>
         <v>-2.9999999999997584E-2</v>
       </c>
@@ -3178,11 +3131,11 @@
       <c r="E9" s="10">
         <v>25.35</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="23">
         <f t="shared" si="0"/>
         <v>-0.11666666666666714</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="23">
         <f t="shared" si="1"/>
         <v>2.0000000000003126E-2</v>
       </c>
@@ -3197,11 +3150,11 @@
       <c r="E10" s="10">
         <v>25.26</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="23">
         <f t="shared" si="0"/>
         <v>-1.6666666666669272E-2</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="23">
         <f t="shared" si="1"/>
         <v>-6.9999999999996732E-2</v>
       </c>
@@ -3216,11 +3169,11 @@
       <c r="E11" s="10">
         <v>25.37</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="23">
         <f t="shared" si="0"/>
         <v>-1.6666666666669272E-2</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="23">
         <f t="shared" si="1"/>
         <v>4.00000000000027E-2</v>
       </c>
@@ -3235,11 +3188,11 @@
       <c r="E12" s="10">
         <v>25.38</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="23">
         <f t="shared" si="0"/>
         <v>8.3333333333332149E-2</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="23">
         <f t="shared" si="1"/>
         <v>5.0000000000000711E-2</v>
       </c>
@@ -3254,11 +3207,11 @@
       <c r="E13" s="10">
         <v>25.35</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="23">
         <f t="shared" si="0"/>
         <v>-6.666666666666643E-2</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="23">
         <f t="shared" si="1"/>
         <v>2.0000000000003126E-2</v>
       </c>
@@ -3273,33 +3226,33 @@
       <c r="E14" s="11">
         <v>25.27</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="23">
         <f t="shared" si="0"/>
         <v>-6.666666666666643E-2</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="23">
         <f t="shared" si="1"/>
         <v>-5.9999999999998721E-2</v>
       </c>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="F15" s="31">
+      <c r="F15" s="26">
         <f>SUM(F3:F14)</f>
         <v>-1.4210854715202004E-14</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="26">
         <f>SUM(G3:G14)</f>
         <v>2.1316282072803006E-14</v>
       </c>
     </row>
     <row r="16" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -3334,11 +3287,11 @@
       <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="24">
         <f>F3^2</f>
         <v>6.9444444444442472E-3</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="25">
         <f>G3^2</f>
         <v>1.0000000000003127E-4</v>
       </c>
@@ -3356,11 +3309,11 @@
       <c r="D20" s="3">
         <v>2</v>
       </c>
-      <c r="F20" s="29">
-        <f t="shared" ref="F20:G33" si="2">F4^2</f>
+      <c r="F20" s="24">
+        <f t="shared" ref="F20:G30" si="2">F4^2</f>
         <v>6.9444444444442472E-3</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3378,11 +3331,11 @@
       <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="24">
         <f t="shared" si="2"/>
         <v>1.1111111111109847E-3</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="25">
         <f t="shared" si="2"/>
         <v>3.9999999999998294E-4</v>
       </c>
@@ -3400,11 +3353,11 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="24">
         <f t="shared" si="2"/>
         <v>1.3611111111111221E-2</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="25">
         <f t="shared" si="2"/>
         <v>9.9999999999960215E-5</v>
       </c>
@@ -3422,11 +3375,11 @@
       <c r="D23" s="3">
         <v>4</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="24">
         <f t="shared" si="2"/>
         <v>1.1111111111109847E-3</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="25">
         <f t="shared" si="2"/>
         <v>2.5000000000000712E-3</v>
       </c>
@@ -3438,15 +3391,15 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="F24" s="29">
+      <c r="D24" s="28"/>
+      <c r="F24" s="24">
         <f t="shared" si="2"/>
         <v>6.9444444444442472E-3</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="25">
         <f t="shared" si="2"/>
         <v>8.9999999999985502E-4</v>
       </c>
@@ -3464,11 +3417,11 @@
       <c r="D25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="24">
         <f t="shared" si="2"/>
         <v>1.3611111111111221E-2</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="25">
         <f t="shared" si="2"/>
         <v>4.0000000000012508E-4</v>
       </c>
@@ -3486,11 +3439,11 @@
       <c r="D26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="24">
         <f t="shared" si="2"/>
         <v>2.7777777777786462E-4</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="25">
         <f t="shared" si="2"/>
         <v>4.8999999999995427E-3</v>
       </c>
@@ -3508,11 +3461,11 @@
       <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="24">
         <f t="shared" si="2"/>
         <v>2.7777777777786462E-4</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="25">
         <f t="shared" si="2"/>
         <v>1.600000000000216E-3</v>
       </c>
@@ -3530,11 +3483,11 @@
       <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="24">
         <f t="shared" si="2"/>
         <v>6.9444444444442472E-3</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="25">
         <f t="shared" si="2"/>
         <v>2.5000000000000712E-3</v>
       </c>
@@ -3546,11 +3499,11 @@
       <c r="D29" s="22">
         <v>1</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="24">
         <f t="shared" si="2"/>
         <v>4.4444444444444132E-3</v>
       </c>
-      <c r="G29" s="30">
+      <c r="G29" s="25">
         <f t="shared" si="2"/>
         <v>4.0000000000012508E-4</v>
       </c>
@@ -3562,11 +3515,11 @@
       <c r="D30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="24">
         <f t="shared" si="2"/>
         <v>4.4444444444444132E-3</v>
       </c>
-      <c r="G30" s="30">
+      <c r="G30" s="25">
         <f t="shared" si="2"/>
         <v>3.5999999999998464E-3</v>
       </c>
@@ -3578,11 +3531,11 @@
       <c r="D31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="23">
         <f>SUM(F19:F30)</f>
         <v>6.6666666666665944E-2</v>
       </c>
-      <c r="G31" s="28">
+      <c r="G31" s="23">
         <f>SUM(G19:G30)</f>
         <v>1.7399999999999829E-2</v>
       </c>
@@ -3594,7 +3547,7 @@
       <c r="D32" s="3">
         <v>1</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="20">
@@ -3603,7 +3556,7 @@
       <c r="D33" s="3">
         <v>2</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="20">
@@ -3626,6 +3579,159 @@
     </row>
     <row r="37" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="11"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="20">
+        <v>25.26</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="20">
+        <v>25.27</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="20">
+        <v>25.3</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="20">
+        <v>25.31</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="20">
+        <v>25.32</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="20">
+        <v>25.33</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="20">
+        <v>25.34</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="20">
+        <v>25.35</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="20">
+        <v>25.37</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="18">
+        <v>25.38</v>
+      </c>
+      <c r="E49" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C26:C37">

</xml_diff>